<commit_message>
Hard link supp-data table to the inputs Excel file
</commit_message>
<xml_diff>
--- a/tex/supp_data/Supp-Data-1-Amplicon-info.xlsx
+++ b/tex/supp_data/Supp-Data-1-Amplicon-info.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ellen/Genetics_Lab_Data/DataAnalysis/california-chinook-microhaps/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eriq/Documents/git-repos/california-chinook-microhaps/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE36DDD2-DE13-AA44-96A3-27A14B840283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A042437D-39EF-864F-9CF1-52F9BA52A920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="3260" windowWidth="47240" windowHeight="22400" xr2:uid="{E56130A1-82B1-034C-9FBF-E21DD198A6C4}"/>
+    <workbookView xWindow="5660" yWindow="760" windowWidth="27080" windowHeight="21580" xr2:uid="{E56130A1-82B1-034C-9FBF-E21DD198A6C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Key" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$T$205</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$V$205</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="1465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2089" uniqueCount="1479">
   <si>
     <t>ACTACAGGCACTCTCCCTGGCTAGAAGGGCAGGATAATAACAAACAAGAGATKATTTAAAGCCAGAGAAGTGATGGGGG</t>
   </si>
@@ -4434,13 +4434,55 @@
   </si>
   <si>
     <t>151, 165, 172</t>
+  </si>
+  <si>
+    <t>LocusType</t>
+  </si>
+  <si>
+    <t>RoSA</t>
+  </si>
+  <si>
+    <t>Sex ID</t>
+  </si>
+  <si>
+    <t>VGLL3</t>
+  </si>
+  <si>
+    <t>Six6</t>
+  </si>
+  <si>
+    <t>LFAR</t>
+  </si>
+  <si>
+    <t>WRAP</t>
+  </si>
+  <si>
+    <t>Microhap</t>
+  </si>
+  <si>
+    <t>SNPtype</t>
+  </si>
+  <si>
+    <t>Original Reference</t>
+  </si>
+  <si>
+    <t>Clemento et al. 2014</t>
+  </si>
+  <si>
+    <t>Thompson et al. 2021</t>
+  </si>
+  <si>
+    <t>This study</t>
+  </si>
+  <si>
+    <t>Waters et al. 2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4471,6 +4513,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4899,27 +4947,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575934F3-73D5-F049-89DB-6A73CBC8D927}">
-  <dimension ref="A1:T205"/>
+  <dimension ref="A1:V205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D189" workbookViewId="0">
-      <selection activeCell="H206" sqref="H206"/>
+    <sheetView tabSelected="1" topLeftCell="I159" workbookViewId="0">
+      <selection activeCell="L209" sqref="L209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" customWidth="1"/>
+    <col min="5" max="7" width="23.6640625" customWidth="1"/>
     <col min="8" max="8" width="29.83203125" customWidth="1"/>
-    <col min="9" max="9" width="61.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="59.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="119.5" style="2" customWidth="1"/>
+    <col min="9" max="9" width="61.5" customWidth="1"/>
+    <col min="10" max="10" width="59.6640625" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.83203125" customWidth="1"/>
+    <col min="13" max="13" width="119.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>98</v>
       </c>
@@ -4950,11 +4999,17 @@
       <c r="J1" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
+        <v>1465</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>1474</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>99</v>
       </c>
@@ -4982,11 +5037,17 @@
       <c r="I2" s="13" t="s">
         <v>334</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="13" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="M2" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -5011,8 +5072,14 @@
       <c r="H3" t="s">
         <v>1293</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K3" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -5037,8 +5104,14 @@
       <c r="H4" t="s">
         <v>1294</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K4" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>102</v>
       </c>
@@ -5063,8 +5136,14 @@
       <c r="H5">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K5" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>103</v>
       </c>
@@ -5089,8 +5168,14 @@
       <c r="H6" t="s">
         <v>1295</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K6" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -5115,8 +5200,14 @@
       <c r="H7">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K7" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>105</v>
       </c>
@@ -5141,8 +5232,14 @@
       <c r="H8" t="s">
         <v>1296</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K8" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>106</v>
       </c>
@@ -5167,8 +5264,14 @@
       <c r="H9" t="s">
         <v>1297</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K9" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>107</v>
       </c>
@@ -5193,8 +5296,14 @@
       <c r="H10" t="s">
         <v>1298</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K10" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>108</v>
       </c>
@@ -5219,8 +5328,14 @@
       <c r="H11" t="s">
         <v>1299</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K11" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>109</v>
       </c>
@@ -5245,8 +5360,14 @@
       <c r="H12" t="s">
         <v>1300</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K12" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>110</v>
       </c>
@@ -5271,8 +5392,14 @@
       <c r="H13" t="s">
         <v>1301</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K13" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>111</v>
       </c>
@@ -5297,8 +5424,14 @@
       <c r="H14">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K14" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>112</v>
       </c>
@@ -5323,8 +5456,14 @@
       <c r="H15" t="s">
         <v>1302</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K15" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>113</v>
       </c>
@@ -5349,8 +5488,14 @@
       <c r="H16" t="s">
         <v>1303</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K16" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>114</v>
       </c>
@@ -5375,8 +5520,14 @@
       <c r="H17" t="s">
         <v>1304</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K17" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>115</v>
       </c>
@@ -5401,8 +5552,14 @@
       <c r="H18">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K18" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>116</v>
       </c>
@@ -5427,8 +5584,14 @@
       <c r="H19" t="s">
         <v>1305</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K19" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
         <v>117</v>
       </c>
@@ -5456,11 +5619,17 @@
       <c r="I20" s="13" t="s">
         <v>330</v>
       </c>
-      <c r="K20" s="14" t="s">
+      <c r="K20" s="13" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="M20" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>118</v>
       </c>
@@ -5485,8 +5654,14 @@
       <c r="H21" t="s">
         <v>1306</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K21" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>119</v>
       </c>
@@ -5511,8 +5686,14 @@
       <c r="H22" t="s">
         <v>1307</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K22" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>120</v>
       </c>
@@ -5537,8 +5718,14 @@
       <c r="H23">
         <v>38</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K23" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>121</v>
       </c>
@@ -5563,8 +5750,14 @@
       <c r="H24">
         <v>34</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K24" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L24" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>122</v>
       </c>
@@ -5589,8 +5782,14 @@
       <c r="H25" t="s">
         <v>1308</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K25" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>123</v>
       </c>
@@ -5615,8 +5814,14 @@
       <c r="H26" t="s">
         <v>1309</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K26" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>124</v>
       </c>
@@ -5641,8 +5846,14 @@
       <c r="H27" t="s">
         <v>1310</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K27" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L27" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
         <v>125</v>
       </c>
@@ -5670,11 +5881,17 @@
       <c r="I28" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="K28" s="14" t="s">
+      <c r="K28" s="13" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L28" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="M28" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>126</v>
       </c>
@@ -5699,8 +5916,14 @@
       <c r="H29" t="s">
         <v>1312</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K29" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L29" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>127</v>
       </c>
@@ -5725,8 +5948,14 @@
       <c r="H30" t="s">
         <v>1313</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K30" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L30" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>128</v>
       </c>
@@ -5751,8 +5980,14 @@
       <c r="H31">
         <v>44</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K31" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L31" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
         <v>129</v>
       </c>
@@ -5780,11 +6015,17 @@
       <c r="I32" s="13" t="s">
         <v>331</v>
       </c>
-      <c r="K32" s="14" t="s">
+      <c r="K32" s="13" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L32" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="M32" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
         <v>130</v>
       </c>
@@ -5812,11 +6053,17 @@
       <c r="I33" s="13" t="s">
         <v>329</v>
       </c>
-      <c r="K33" s="14" t="s">
+      <c r="K33" s="13" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L33" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="M33" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>131</v>
       </c>
@@ -5841,8 +6088,14 @@
       <c r="H34">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K34" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L34" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>132</v>
       </c>
@@ -5867,8 +6120,14 @@
       <c r="H35" t="s">
         <v>1315</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K35" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L35" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>133</v>
       </c>
@@ -5893,8 +6152,14 @@
       <c r="H36">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K36" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L36" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>134</v>
       </c>
@@ -5919,8 +6184,14 @@
       <c r="H37" t="s">
         <v>1316</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K37" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L37" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="13" t="s">
         <v>135</v>
       </c>
@@ -5948,11 +6219,17 @@
       <c r="I38" s="13" t="s">
         <v>332</v>
       </c>
-      <c r="K38" s="14" t="s">
+      <c r="K38" s="13" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L38" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="M38" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>136</v>
       </c>
@@ -5977,8 +6254,14 @@
       <c r="H39" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K39" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L39" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>137</v>
       </c>
@@ -6009,11 +6292,17 @@
       <c r="J40" s="9" t="s">
         <v>1272</v>
       </c>
-      <c r="K40" s="10" t="s">
+      <c r="K40" s="9" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L40" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="M40" s="10" t="s">
         <v>1291</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>138</v>
       </c>
@@ -6038,8 +6327,14 @@
       <c r="H41" t="s">
         <v>1320</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" s="20" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K41" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L41" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" s="20" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="s">
         <v>139</v>
       </c>
@@ -6070,11 +6365,17 @@
       <c r="J42" s="20" t="s">
         <v>1271</v>
       </c>
-      <c r="K42" s="21" t="s">
+      <c r="K42" s="20" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L42" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="M42" s="21" t="s">
         <v>1277</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>140</v>
       </c>
@@ -6099,8 +6400,14 @@
       <c r="H43" t="s">
         <v>1321</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K43" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L43" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>141</v>
       </c>
@@ -6125,8 +6432,14 @@
       <c r="H44" t="s">
         <v>1315</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K44" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L44" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>142</v>
       </c>
@@ -6151,8 +6464,14 @@
       <c r="H45" t="s">
         <v>1322</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K45" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L45" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>143</v>
       </c>
@@ -6177,8 +6496,14 @@
       <c r="H46">
         <v>35</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K46" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L46" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>144</v>
       </c>
@@ -6203,8 +6528,14 @@
       <c r="H47" t="s">
         <v>1323</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K47" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L47" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>145</v>
       </c>
@@ -6229,8 +6560,14 @@
       <c r="H48">
         <v>44</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K48" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L48" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>146</v>
       </c>
@@ -6255,8 +6592,14 @@
       <c r="H49">
         <v>44</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K49" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L49" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="13" t="s">
         <v>147</v>
       </c>
@@ -6284,11 +6627,17 @@
       <c r="I50" s="13" t="s">
         <v>333</v>
       </c>
-      <c r="K50" s="14" t="s">
+      <c r="K50" s="13" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L50" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="M50" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>148</v>
       </c>
@@ -6313,8 +6662,14 @@
       <c r="H51" t="s">
         <v>1325</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K51" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L51" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>149</v>
       </c>
@@ -6339,8 +6694,14 @@
       <c r="H52" t="s">
         <v>1326</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K52" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L52" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>150</v>
       </c>
@@ -6365,8 +6726,14 @@
       <c r="H53" t="s">
         <v>1327</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K53" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L53" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>151</v>
       </c>
@@ -6391,8 +6758,14 @@
       <c r="H54" t="s">
         <v>1328</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K54" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L54" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>152</v>
       </c>
@@ -6417,8 +6790,14 @@
       <c r="H55" t="s">
         <v>1329</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K55" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L55" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>153</v>
       </c>
@@ -6443,8 +6822,14 @@
       <c r="H56">
         <v>39</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K56" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L56" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>154</v>
       </c>
@@ -6469,8 +6854,14 @@
       <c r="H57" t="s">
         <v>1330</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K57" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L57" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>155</v>
       </c>
@@ -6495,8 +6886,14 @@
       <c r="H58">
         <v>40</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K58" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L58" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>156</v>
       </c>
@@ -6521,8 +6918,14 @@
       <c r="H59" t="s">
         <v>1331</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K59" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L59" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>157</v>
       </c>
@@ -6547,8 +6950,14 @@
       <c r="H60" t="s">
         <v>1332</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K60" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L60" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>158</v>
       </c>
@@ -6573,8 +6982,14 @@
       <c r="H61" t="s">
         <v>1333</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K61" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L61" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>159</v>
       </c>
@@ -6599,8 +7014,14 @@
       <c r="H62" t="s">
         <v>1334</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K62" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L62" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>160</v>
       </c>
@@ -6625,8 +7046,14 @@
       <c r="H63" t="s">
         <v>1335</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K63" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L63" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
         <v>161</v>
       </c>
@@ -6654,11 +7081,17 @@
       <c r="J64" s="11" t="s">
         <v>1273</v>
       </c>
-      <c r="K64" s="12" t="s">
+      <c r="K64" s="11" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L64" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="M64" s="12" t="s">
         <v>1280</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>162</v>
       </c>
@@ -6683,8 +7116,14 @@
       <c r="H65">
         <v>43</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K65" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L65" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>163</v>
       </c>
@@ -6709,8 +7148,14 @@
       <c r="H66" t="s">
         <v>1337</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K66" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L66" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>164</v>
       </c>
@@ -6735,8 +7180,14 @@
       <c r="H67">
         <v>52</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K67" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L67" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>165</v>
       </c>
@@ -6761,8 +7212,14 @@
       <c r="H68">
         <v>32</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K68" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L68" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>166</v>
       </c>
@@ -6787,8 +7244,14 @@
       <c r="H69" t="s">
         <v>1338</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K69" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L69" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>167</v>
       </c>
@@ -6813,8 +7276,14 @@
       <c r="H70">
         <v>35</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K70" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L70" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>168</v>
       </c>
@@ -6839,8 +7308,14 @@
       <c r="H71" t="s">
         <v>1339</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K71" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L71" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>169</v>
       </c>
@@ -6865,8 +7340,14 @@
       <c r="H72" t="s">
         <v>1340</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K72" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L72" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="13" t="s">
         <v>170</v>
       </c>
@@ -6894,11 +7375,17 @@
       <c r="I73" s="13" t="s">
         <v>335</v>
       </c>
-      <c r="K73" s="14" t="s">
+      <c r="K73" s="13" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L73" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="M73" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>171</v>
       </c>
@@ -6923,8 +7410,14 @@
       <c r="H74" t="s">
         <v>1342</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K74" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L74" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>172</v>
       </c>
@@ -6949,8 +7442,14 @@
       <c r="H75" t="s">
         <v>1343</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K75" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L75" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>173</v>
       </c>
@@ -6975,8 +7474,14 @@
       <c r="H76">
         <v>56</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K76" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L76" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>174</v>
       </c>
@@ -7001,8 +7506,14 @@
       <c r="H77">
         <v>55</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K77" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L77" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>175</v>
       </c>
@@ -7027,8 +7538,14 @@
       <c r="H78" t="s">
         <v>1344</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K78" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L78" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>176</v>
       </c>
@@ -7053,8 +7570,14 @@
       <c r="H79">
         <v>68</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K79" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L79" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>177</v>
       </c>
@@ -7079,8 +7602,14 @@
       <c r="H80">
         <v>49</v>
       </c>
-    </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="K80" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L80" s="13" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="81" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>178</v>
       </c>
@@ -7105,8 +7634,14 @@
       <c r="H81" t="s">
         <v>1345</v>
       </c>
-    </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="K81" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L81" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="82" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>179</v>
       </c>
@@ -7131,8 +7666,14 @@
       <c r="H82" t="s">
         <v>1346</v>
       </c>
-    </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="K82" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L82" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="83" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>180</v>
       </c>
@@ -7157,8 +7698,14 @@
       <c r="H83" t="s">
         <v>1347</v>
       </c>
-    </row>
-    <row r="84" spans="1:20" s="7" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="K83" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L83" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="84" spans="1:22" s="7" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
         <v>181</v>
       </c>
@@ -7183,11 +7730,17 @@
       <c r="H84" s="7" t="s">
         <v>1348</v>
       </c>
-      <c r="K84" s="8" t="s">
+      <c r="K84" s="7" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L84" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M84" s="8" t="s">
         <v>1275</v>
       </c>
     </row>
-    <row r="85" spans="1:20" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:22" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
         <v>182</v>
       </c>
@@ -7215,11 +7768,17 @@
       <c r="J85" s="11" t="s">
         <v>1274</v>
       </c>
-      <c r="K85" s="12" t="s">
+      <c r="K85" s="11" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L85" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M85" s="12" t="s">
         <v>1280</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>183</v>
       </c>
@@ -7244,8 +7803,14 @@
       <c r="H86" t="s">
         <v>1350</v>
       </c>
-    </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="K86" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L86" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="87" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>184</v>
       </c>
@@ -7270,8 +7835,14 @@
       <c r="H87" t="s">
         <v>1351</v>
       </c>
-    </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="K87" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L87" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="88" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>185</v>
       </c>
@@ -7296,8 +7867,14 @@
       <c r="H88" t="s">
         <v>1352</v>
       </c>
-    </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="K88" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L88" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="89" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>186</v>
       </c>
@@ -7322,8 +7899,14 @@
       <c r="H89" t="s">
         <v>1353</v>
       </c>
-    </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="K89" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L89" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="90" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>187</v>
       </c>
@@ -7348,9 +7931,15 @@
       <c r="H90" t="s">
         <v>1354</v>
       </c>
-      <c r="N90" s="1"/>
-    </row>
-    <row r="91" spans="1:20" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K90" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L90" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="P90" s="1"/>
+    </row>
+    <row r="91" spans="1:22" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="13" t="s">
         <v>188</v>
       </c>
@@ -7378,18 +7967,24 @@
       <c r="I91" s="13" t="s">
         <v>336</v>
       </c>
-      <c r="K91" s="14" t="s">
+      <c r="K91" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L91" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M91" s="14" t="s">
         <v>1278</v>
       </c>
-      <c r="N91" s="15"/>
-      <c r="O91" s="15"/>
       <c r="P91" s="15"/>
       <c r="Q91" s="15"/>
       <c r="R91" s="15"/>
       <c r="S91" s="15"/>
       <c r="T91" s="15"/>
-    </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U91" s="15"/>
+      <c r="V91" s="15"/>
+    </row>
+    <row r="92" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>189</v>
       </c>
@@ -7414,8 +8009,14 @@
       <c r="H92" t="s">
         <v>1356</v>
       </c>
-    </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="K92" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L92" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="93" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>190</v>
       </c>
@@ -7440,8 +8041,14 @@
       <c r="H93" t="s">
         <v>1357</v>
       </c>
-    </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="K93" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L93" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="94" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>191</v>
       </c>
@@ -7466,8 +8073,14 @@
       <c r="H94" t="s">
         <v>1358</v>
       </c>
-    </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="K94" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L94" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="95" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>192</v>
       </c>
@@ -7492,8 +8105,14 @@
       <c r="H95" t="s">
         <v>1359</v>
       </c>
-    </row>
-    <row r="96" spans="1:20" s="16" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="K95" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L95" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="96" spans="1:22" s="16" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A96" s="16" t="s">
         <v>193</v>
       </c>
@@ -7524,11 +8143,17 @@
       <c r="J96" s="16" t="s">
         <v>1286</v>
       </c>
-      <c r="K96" s="17" t="s">
+      <c r="K96" s="16" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L96" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M96" s="17" t="s">
         <v>1290</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>194</v>
       </c>
@@ -7553,8 +8178,14 @@
       <c r="H97" t="s">
         <v>1361</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K97" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L97" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="13" t="s">
         <v>195</v>
       </c>
@@ -7582,11 +8213,17 @@
       <c r="I98" s="13" t="s">
         <v>338</v>
       </c>
-      <c r="K98" s="14" t="s">
+      <c r="K98" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L98" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M98" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>196</v>
       </c>
@@ -7611,8 +8248,14 @@
       <c r="H99" t="s">
         <v>1363</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K99" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L99" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>197</v>
       </c>
@@ -7637,8 +8280,14 @@
       <c r="H100" t="s">
         <v>1364</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K100" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L100" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>198</v>
       </c>
@@ -7663,8 +8312,14 @@
       <c r="H101" t="s">
         <v>1365</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K101" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L101" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>199</v>
       </c>
@@ -7689,8 +8344,14 @@
       <c r="H102" t="s">
         <v>1366</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K102" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L102" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>200</v>
       </c>
@@ -7715,8 +8376,14 @@
       <c r="H103" t="s">
         <v>1367</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K103" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L103" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="13" t="s">
         <v>201</v>
       </c>
@@ -7744,11 +8411,17 @@
       <c r="I104" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="K104" s="14" t="s">
+      <c r="K104" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L104" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M104" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>202</v>
       </c>
@@ -7773,8 +8446,14 @@
       <c r="H105" t="s">
         <v>1369</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K105" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L105" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>203</v>
       </c>
@@ -7799,8 +8478,14 @@
       <c r="H106" t="s">
         <v>1370</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K106" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L106" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>204</v>
       </c>
@@ -7825,8 +8510,14 @@
       <c r="H107" t="s">
         <v>1371</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K107" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L107" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>205</v>
       </c>
@@ -7851,8 +8542,14 @@
       <c r="H108" t="s">
         <v>1372</v>
       </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K108" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L108" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>206</v>
       </c>
@@ -7877,8 +8574,14 @@
       <c r="H109" t="s">
         <v>1373</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K109" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L109" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>207</v>
       </c>
@@ -7903,8 +8606,14 @@
       <c r="H110" t="s">
         <v>1374</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K110" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L110" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>208</v>
       </c>
@@ -7929,8 +8638,14 @@
       <c r="H111" t="s">
         <v>1375</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K111" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L111" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>209</v>
       </c>
@@ -7955,8 +8670,14 @@
       <c r="H112" t="s">
         <v>1376</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K112" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L112" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="13" t="s">
         <v>210</v>
       </c>
@@ -7984,11 +8705,17 @@
       <c r="I113" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="K113" s="14" t="s">
+      <c r="K113" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L113" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M113" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>211</v>
       </c>
@@ -8013,8 +8740,14 @@
       <c r="H114" t="s">
         <v>1378</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K114" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L114" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>212</v>
       </c>
@@ -8039,8 +8772,14 @@
       <c r="H115" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K115" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L115" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="13" t="s">
         <v>213</v>
       </c>
@@ -8068,11 +8807,17 @@
       <c r="I116" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="K116" s="14" t="s">
+      <c r="K116" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L116" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M116" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>214</v>
       </c>
@@ -8097,8 +8842,14 @@
       <c r="H117" t="s">
         <v>1381</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K117" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L117" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>215</v>
       </c>
@@ -8123,8 +8874,14 @@
       <c r="H118" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K118" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L118" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>216</v>
       </c>
@@ -8149,8 +8906,14 @@
       <c r="H119" t="s">
         <v>1383</v>
       </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K119" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L119" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>217</v>
       </c>
@@ -8175,8 +8938,14 @@
       <c r="H120" t="s">
         <v>1384</v>
       </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K120" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L120" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>218</v>
       </c>
@@ -8201,8 +8970,14 @@
       <c r="H121" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K121" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L121" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>219</v>
       </c>
@@ -8227,8 +9002,14 @@
       <c r="H122" t="s">
         <v>1386</v>
       </c>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K122" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L122" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>220</v>
       </c>
@@ -8253,8 +9034,14 @@
       <c r="H123" t="s">
         <v>1387</v>
       </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K123" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L123" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>221</v>
       </c>
@@ -8279,8 +9066,14 @@
       <c r="H124" t="s">
         <v>1388</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K124" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L124" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="13" t="s">
         <v>222</v>
       </c>
@@ -8308,11 +9101,17 @@
       <c r="I125" s="13" t="s">
         <v>341</v>
       </c>
-      <c r="K125" s="14" t="s">
+      <c r="K125" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L125" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M125" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>223</v>
       </c>
@@ -8337,8 +9136,14 @@
       <c r="H126" t="s">
         <v>1390</v>
       </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K126" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L126" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>224</v>
       </c>
@@ -8363,8 +9168,14 @@
       <c r="H127" t="s">
         <v>1391</v>
       </c>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K127" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L127" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>225</v>
       </c>
@@ -8389,8 +9200,14 @@
       <c r="H128" t="s">
         <v>1392</v>
       </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K128" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L128" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>226</v>
       </c>
@@ -8415,8 +9232,14 @@
       <c r="H129" t="s">
         <v>1393</v>
       </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K129" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L129" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>227</v>
       </c>
@@ -8441,8 +9264,14 @@
       <c r="H130" t="s">
         <v>1394</v>
       </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K130" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L130" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>228</v>
       </c>
@@ -8467,8 +9296,14 @@
       <c r="H131" t="s">
         <v>1395</v>
       </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K131" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L131" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>229</v>
       </c>
@@ -8493,8 +9328,14 @@
       <c r="H132" t="s">
         <v>1396</v>
       </c>
-    </row>
-    <row r="133" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K132" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L132" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="13" t="s">
         <v>230</v>
       </c>
@@ -8522,11 +9363,17 @@
       <c r="I133" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="K133" s="14" t="s">
+      <c r="K133" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L133" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M133" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>231</v>
       </c>
@@ -8551,8 +9398,14 @@
       <c r="H134" t="s">
         <v>1398</v>
       </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K134" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L134" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>232</v>
       </c>
@@ -8577,8 +9430,14 @@
       <c r="H135" t="s">
         <v>1399</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K135" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L135" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>233</v>
       </c>
@@ -8603,8 +9462,14 @@
       <c r="H136" t="s">
         <v>1400</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K136" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L136" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>234</v>
       </c>
@@ -8629,8 +9494,14 @@
       <c r="H137" t="s">
         <v>1401</v>
       </c>
-    </row>
-    <row r="138" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K137" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L137" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="13" t="s">
         <v>235</v>
       </c>
@@ -8658,11 +9529,17 @@
       <c r="I138" s="13" t="s">
         <v>350</v>
       </c>
-      <c r="K138" s="14" t="s">
+      <c r="K138" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L138" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M138" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="139" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="13" t="s">
         <v>236</v>
       </c>
@@ -8690,11 +9567,17 @@
       <c r="I139" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="K139" s="14" t="s">
+      <c r="K139" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L139" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M139" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>237</v>
       </c>
@@ -8719,8 +9602,14 @@
       <c r="H140" t="s">
         <v>1404</v>
       </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K140" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L140" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>238</v>
       </c>
@@ -8745,8 +9634,14 @@
       <c r="H141" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K141" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L141" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>239</v>
       </c>
@@ -8771,8 +9666,14 @@
       <c r="H142" t="s">
         <v>1406</v>
       </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K142" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L142" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>240</v>
       </c>
@@ -8797,8 +9698,14 @@
       <c r="H143" t="s">
         <v>1407</v>
       </c>
-    </row>
-    <row r="144" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K143" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L143" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="13" t="s">
         <v>241</v>
       </c>
@@ -8826,11 +9733,17 @@
       <c r="I144" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="K144" s="14" t="s">
+      <c r="K144" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L144" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M144" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>242</v>
       </c>
@@ -8855,8 +9768,14 @@
       <c r="H145" t="s">
         <v>1409</v>
       </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K145" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L145" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>243</v>
       </c>
@@ -8881,8 +9800,14 @@
       <c r="H146" t="s">
         <v>1410</v>
       </c>
-    </row>
-    <row r="147" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K146" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L146" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" s="13" t="s">
         <v>244</v>
       </c>
@@ -8910,11 +9835,17 @@
       <c r="I147" s="13" t="s">
         <v>345</v>
       </c>
-      <c r="K147" s="14" t="s">
+      <c r="K147" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L147" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M147" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="148" spans="1:11" s="18" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:13" s="18" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A148" s="18" t="s">
         <v>245</v>
       </c>
@@ -8939,11 +9870,17 @@
       <c r="H148" s="18" t="s">
         <v>1412</v>
       </c>
-      <c r="K148" s="19" t="s">
+      <c r="K148" s="18" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L148" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M148" s="19" t="s">
         <v>1287</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>246</v>
       </c>
@@ -8968,8 +9905,14 @@
       <c r="H149" t="s">
         <v>1413</v>
       </c>
-    </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K149" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L149" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>247</v>
       </c>
@@ -8994,8 +9937,14 @@
       <c r="H150" t="s">
         <v>1414</v>
       </c>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K150" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L150" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>248</v>
       </c>
@@ -9020,8 +9969,14 @@
       <c r="H151" t="s">
         <v>1415</v>
       </c>
-    </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K151" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L151" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>249</v>
       </c>
@@ -9046,8 +10001,14 @@
       <c r="H152" t="s">
         <v>1416</v>
       </c>
-    </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K152" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L152" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>250</v>
       </c>
@@ -9072,8 +10033,14 @@
       <c r="H153" t="s">
         <v>1417</v>
       </c>
-    </row>
-    <row r="154" spans="1:11" s="7" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="K153" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L153" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" s="7" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A154" s="7" t="s">
         <v>251</v>
       </c>
@@ -9098,11 +10065,17 @@
       <c r="H154" s="7" t="s">
         <v>1418</v>
       </c>
-      <c r="K154" s="8" t="s">
+      <c r="K154" s="7" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L154" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M154" s="8" t="s">
         <v>1276</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>252</v>
       </c>
@@ -9127,8 +10100,14 @@
       <c r="H155" t="s">
         <v>1419</v>
       </c>
-    </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K155" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L155" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>253</v>
       </c>
@@ -9153,8 +10132,14 @@
       <c r="H156" t="s">
         <v>1420</v>
       </c>
-    </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K156" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L156" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>254</v>
       </c>
@@ -9179,8 +10164,14 @@
       <c r="H157" t="s">
         <v>1421</v>
       </c>
-    </row>
-    <row r="158" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K157" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L157" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A158" s="13" t="s">
         <v>255</v>
       </c>
@@ -9208,11 +10199,17 @@
       <c r="I158" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="K158" s="14" t="s">
+      <c r="K158" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L158" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M158" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>256</v>
       </c>
@@ -9237,8 +10234,14 @@
       <c r="H159" t="s">
         <v>1423</v>
       </c>
-    </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K159" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L159" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>257</v>
       </c>
@@ -9263,8 +10266,14 @@
       <c r="H160" t="s">
         <v>1424</v>
       </c>
-    </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K160" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L160" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>258</v>
       </c>
@@ -9289,8 +10298,14 @@
       <c r="H161" t="s">
         <v>1425</v>
       </c>
-    </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K161" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L161" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>259</v>
       </c>
@@ -9315,8 +10330,14 @@
       <c r="H162" t="s">
         <v>1426</v>
       </c>
-    </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K162" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L162" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>260</v>
       </c>
@@ -9341,8 +10362,14 @@
       <c r="H163" t="s">
         <v>1427</v>
       </c>
-    </row>
-    <row r="164" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K163" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L163" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A164" s="13" t="s">
         <v>261</v>
       </c>
@@ -9370,11 +10397,17 @@
       <c r="I164" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="K164" s="14" t="s">
+      <c r="K164" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L164" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M164" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>262</v>
       </c>
@@ -9399,8 +10432,14 @@
       <c r="H165" t="s">
         <v>1429</v>
       </c>
-    </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K165" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L165" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>263</v>
       </c>
@@ -9425,8 +10464,14 @@
       <c r="H166" t="s">
         <v>1430</v>
       </c>
-    </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K166" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L166" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>264</v>
       </c>
@@ -9451,8 +10496,14 @@
       <c r="H167" t="s">
         <v>1431</v>
       </c>
-    </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K167" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L167" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>265</v>
       </c>
@@ -9477,8 +10528,14 @@
       <c r="H168" t="s">
         <v>1432</v>
       </c>
-    </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K168" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L168" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>266</v>
       </c>
@@ -9503,8 +10560,14 @@
       <c r="H169" t="s">
         <v>1433</v>
       </c>
-    </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K169" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L169" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>267</v>
       </c>
@@ -9529,8 +10592,14 @@
       <c r="H170" t="s">
         <v>1434</v>
       </c>
-    </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K170" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L170" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>268</v>
       </c>
@@ -9555,8 +10624,14 @@
       <c r="H171" t="s">
         <v>1435</v>
       </c>
-    </row>
-    <row r="172" spans="1:11" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="K171" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L171" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A172" s="13" t="s">
         <v>269</v>
       </c>
@@ -9584,11 +10659,17 @@
       <c r="I172" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="K172" s="14" t="s">
+      <c r="K172" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L172" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M172" s="14" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>270</v>
       </c>
@@ -9613,8 +10694,14 @@
       <c r="H173" t="s">
         <v>1437</v>
       </c>
-    </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K173" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L173" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>271</v>
       </c>
@@ -9639,8 +10726,14 @@
       <c r="H174" t="s">
         <v>1438</v>
       </c>
-    </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K174" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L174" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>272</v>
       </c>
@@ -9665,8 +10758,14 @@
       <c r="H175" t="s">
         <v>1439</v>
       </c>
-    </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K175" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L175" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>273</v>
       </c>
@@ -9691,8 +10790,14 @@
       <c r="H176" t="s">
         <v>1440</v>
       </c>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K176" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L176" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>274</v>
       </c>
@@ -9717,8 +10822,14 @@
       <c r="H177" t="s">
         <v>1441</v>
       </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K177" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L177" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>275</v>
       </c>
@@ -9743,8 +10854,14 @@
       <c r="H178" t="s">
         <v>1442</v>
       </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K178" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L178" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>276</v>
       </c>
@@ -9769,8 +10886,14 @@
       <c r="H179" t="s">
         <v>1443</v>
       </c>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K179" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L179" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>277</v>
       </c>
@@ -9795,8 +10918,14 @@
       <c r="H180" t="s">
         <v>1444</v>
       </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K180" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L180" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>278</v>
       </c>
@@ -9821,8 +10950,14 @@
       <c r="H181" t="s">
         <v>1445</v>
       </c>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K181" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L181" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>279</v>
       </c>
@@ -9847,8 +10982,14 @@
       <c r="H182" t="s">
         <v>1446</v>
       </c>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K182" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L182" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>280</v>
       </c>
@@ -9873,8 +11014,14 @@
       <c r="H183" t="s">
         <v>1447</v>
       </c>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K183" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L183" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>281</v>
       </c>
@@ -9899,8 +11046,14 @@
       <c r="H184" t="s">
         <v>1448</v>
       </c>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K184" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L184" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>282</v>
       </c>
@@ -9925,8 +11078,14 @@
       <c r="H185" t="s">
         <v>1449</v>
       </c>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K185" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L185" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>283</v>
       </c>
@@ -9951,8 +11110,14 @@
       <c r="H186" t="s">
         <v>1450</v>
       </c>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K186" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L186" s="13" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>284</v>
       </c>
@@ -9977,8 +11142,15 @@
       <c r="H187" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K187" t="s">
+        <v>1466</v>
+      </c>
+      <c r="L187" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M187"/>
+    </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>285</v>
       </c>
@@ -10003,8 +11175,15 @@
       <c r="H188" t="s">
         <v>1452</v>
       </c>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K188" t="s">
+        <v>1466</v>
+      </c>
+      <c r="L188" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M188"/>
+    </row>
+    <row r="189" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>286</v>
       </c>
@@ -10029,8 +11208,15 @@
       <c r="H189" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K189" t="s">
+        <v>1466</v>
+      </c>
+      <c r="L189" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M189"/>
+    </row>
+    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>287</v>
       </c>
@@ -10055,8 +11241,15 @@
       <c r="H190" t="s">
         <v>1454</v>
       </c>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K190" t="s">
+        <v>1466</v>
+      </c>
+      <c r="L190" t="s">
+        <v>1477</v>
+      </c>
+      <c r="M190"/>
+    </row>
+    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>288</v>
       </c>
@@ -10081,8 +11274,15 @@
       <c r="H191" t="s">
         <v>1455</v>
       </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K191" t="s">
+        <v>1466</v>
+      </c>
+      <c r="L191" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M191"/>
+    </row>
+    <row r="192" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>289</v>
       </c>
@@ -10107,8 +11307,15 @@
       <c r="H192" t="s">
         <v>1456</v>
       </c>
-    </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K192" t="s">
+        <v>1466</v>
+      </c>
+      <c r="L192" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M192"/>
+    </row>
+    <row r="193" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>290</v>
       </c>
@@ -10133,8 +11340,15 @@
       <c r="H193" t="s">
         <v>1457</v>
       </c>
-    </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K193" t="s">
+        <v>1466</v>
+      </c>
+      <c r="L193" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="M193"/>
+    </row>
+    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>291</v>
       </c>
@@ -10159,8 +11373,15 @@
       <c r="H194" t="s">
         <v>1458</v>
       </c>
-    </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K194" t="s">
+        <v>1466</v>
+      </c>
+      <c r="L194" t="s">
+        <v>1477</v>
+      </c>
+      <c r="M194"/>
+    </row>
+    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>292</v>
       </c>
@@ -10185,8 +11406,15 @@
       <c r="H195" t="s">
         <v>1459</v>
       </c>
-    </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K195" t="s">
+        <v>1466</v>
+      </c>
+      <c r="L195" t="s">
+        <v>1477</v>
+      </c>
+      <c r="M195"/>
+    </row>
+    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>293</v>
       </c>
@@ -10211,8 +11439,15 @@
       <c r="H196" t="s">
         <v>1460</v>
       </c>
-    </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K196" t="s">
+        <v>1466</v>
+      </c>
+      <c r="L196" t="s">
+        <v>1477</v>
+      </c>
+      <c r="M196"/>
+    </row>
+    <row r="197" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>294</v>
       </c>
@@ -10232,10 +11467,13 @@
         <v>89</v>
       </c>
       <c r="K197" t="s">
+        <v>1467</v>
+      </c>
+      <c r="M197" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>295</v>
       </c>
@@ -10262,8 +11500,15 @@
       </c>
       <c r="I198" s="3"/>
       <c r="J198" s="3"/>
-    </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K198" t="s">
+        <v>1469</v>
+      </c>
+      <c r="L198" t="s">
+        <v>1478</v>
+      </c>
+      <c r="M198"/>
+    </row>
+    <row r="199" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>296</v>
       </c>
@@ -10290,8 +11535,15 @@
       </c>
       <c r="I199" s="3"/>
       <c r="J199" s="3"/>
-    </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K199" t="s">
+        <v>1469</v>
+      </c>
+      <c r="L199" t="s">
+        <v>1478</v>
+      </c>
+      <c r="M199"/>
+    </row>
+    <row r="200" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>297</v>
       </c>
@@ -10318,8 +11570,15 @@
       </c>
       <c r="I200" s="3"/>
       <c r="J200" s="3"/>
-    </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K200" t="s">
+        <v>1468</v>
+      </c>
+      <c r="L200" t="s">
+        <v>1478</v>
+      </c>
+      <c r="M200"/>
+    </row>
+    <row r="201" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>298</v>
       </c>
@@ -10346,8 +11605,14 @@
       </c>
       <c r="I201" s="4"/>
       <c r="J201" s="4"/>
-    </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K201" t="s">
+        <v>1470</v>
+      </c>
+      <c r="L201" t="s">
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="202" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>299</v>
       </c>
@@ -10374,8 +11639,14 @@
       </c>
       <c r="I202" s="4"/>
       <c r="J202" s="4"/>
-    </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K202" t="s">
+        <v>1470</v>
+      </c>
+      <c r="L202" t="s">
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="203" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>300</v>
       </c>
@@ -10400,8 +11671,14 @@
       <c r="H203">
         <v>151</v>
       </c>
-    </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K203" t="s">
+        <v>1471</v>
+      </c>
+      <c r="L203" t="s">
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="204" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>301</v>
       </c>
@@ -10426,8 +11703,14 @@
       <c r="H204" t="s">
         <v>1463</v>
       </c>
-    </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K204" t="s">
+        <v>1471</v>
+      </c>
+      <c r="L204" t="s">
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="205" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>302</v>
       </c>
@@ -10452,9 +11735,15 @@
       <c r="H205" t="s">
         <v>1464</v>
       </c>
+      <c r="K205" t="s">
+        <v>1471</v>
+      </c>
+      <c r="L205" t="s">
+        <v>1477</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T205" xr:uid="{575934F3-73D5-F049-89DB-6A73CBC8D927}"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>